<commit_message>
Rework Python scripts + Multiselect grouping + Toggle button edges same category + Bug fixes
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeel\Google Drive\master_project_and_literature_study\literature_study\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeel\Google Drive\master_project_and_literature_study\literature_study\visualization_DTs_ecosystems\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F7E9BD-D080-4DEF-8B28-49CD0E24D45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD4F502-C52D-48ED-BA93-A2DEEE4D5446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="13350" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="literature" sheetId="1" r:id="rId1"/>
+    <sheet name="assessment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="234">
   <si>
     <t>Type Paper</t>
   </si>
@@ -616,12 +617,127 @@
   <si>
     <t>https://onlinelibrary.wiley.com/doi/full/10.1002/cnm.3600</t>
   </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Data regarding size, shape, and other relevant information of an object, represented in 3D.</t>
+  </si>
+  <si>
+    <t>Data revolving around a specific location in the real world, e.g. GIS data.</t>
+  </si>
+  <si>
+    <t>Data acquired from sensors, e.g. temperature.</t>
+  </si>
+  <si>
+    <t>Data regarding previous events about a subject.</t>
+  </si>
+  <si>
+    <t>Data generated during system operation, e.g. real-time data.</t>
+  </si>
+  <si>
+    <t>Data generated from computer simulations, e.g. fluid dynamics simulation.</t>
+  </si>
+  <si>
+    <t>Data providing additional information about other data, e.g. file format or source.</t>
+  </si>
+  <si>
+    <t>Information about characteristics of a specific geographic area, e.g. vegetation or rainfall.</t>
+  </si>
+  <si>
+    <t>Data involving living organisms, e.g. plants, bacteria, and human beings.</t>
+  </si>
+  <si>
+    <t>Data involving nonliving that affect organisms, e.g. climate, water, and atmosphere.</t>
+  </si>
+  <si>
+    <t>Data regarding interaction between individuals.</t>
+  </si>
+  <si>
+    <t>Immersive Visualization Techniques</t>
+  </si>
+  <si>
+    <t>2D plots</t>
+  </si>
+  <si>
+    <t>A collection of two-dimensional visualization techniques</t>
+  </si>
+  <si>
+    <t>Game Engines</t>
+  </si>
+  <si>
+    <t>Modeling Software</t>
+  </si>
+  <si>
+    <t>Javascript Libaries/Frameworks/Packages</t>
+  </si>
+  <si>
+    <t>Web-based Libaries/Frameworks/Packages</t>
+  </si>
+  <si>
+    <t>Immersive Head-Mounted Displays</t>
+  </si>
+  <si>
+    <t>Computing Power</t>
+  </si>
+  <si>
+    <t>Continuous Improvement: how decisions are made for improvements, simulation</t>
+  </si>
+  <si>
+    <t>accuracy/ high fidelity: a good enough view of the model</t>
+  </si>
+  <si>
+    <t>obtrusivenes, visibility, transparancy ease of perception for human beings, from dasboards to 3D, etc, transparancy</t>
+  </si>
+  <si>
+    <t>granularity: indicates the detail level of the model, which can help us to look into the future scenarios in different fidelities, zooming in and out.</t>
+  </si>
+  <si>
+    <t>Standardization alignment in understnading (different domains, stakeholders, etc.),</t>
+  </si>
+  <si>
+    <t>economic value proposition</t>
+  </si>
+  <si>
+    <t>usability/education/ (how well can people operate and understand it?)</t>
+  </si>
+  <si>
+    <t>safety/certifactes/verifications (how safe?)</t>
+  </si>
+  <si>
+    <t>collaboration</t>
+  </si>
+  <si>
+    <t>real-time: low latency, data compression</t>
+  </si>
+  <si>
+    <t>Network Connectivity 
+(connected to the network through Bluetooth, Wi-Fi, etc.)</t>
+  </si>
+  <si>
+    <t>Data Capacity: enough to support DT, collection/ scalability</t>
+  </si>
+  <si>
+    <t>integration seamless integration of data into system, all data</t>
+  </si>
+  <si>
+    <t>security: privacy, integrity, encryption, authentication, blockchain</t>
+  </si>
+  <si>
+    <t>Reliability/robustness/resilience/availability</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,6 +768,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -689,7 +813,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -727,12 +851,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -797,6 +930,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1080,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT926"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71938,4 +72076,714 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId82"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99F4AA7-9738-4229-9559-79AF3E628185}">
+  <dimension ref="A1:S66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>211</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>214</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>215</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>215</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>215</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" t="s">
+        <v>216</v>
+      </c>
+      <c r="C47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
+        <v>215</v>
+      </c>
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" t="s">
+        <v>216</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>217</v>
+      </c>
+      <c r="C62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>217</v>
+      </c>
+      <c r="C64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>217</v>
+      </c>
+      <c r="C66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update README + Added Makefile
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeel\Google Drive\master_project_and_literature_study\literature_study\visualization_DTs_ecosystems\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD4F502-C52D-48ED-BA93-A2DEEE4D5446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBE5B6E-511C-4D6D-A85D-B8A12DC5AC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="13350" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
@@ -72083,8 +72083,8 @@
   <dimension ref="A1:S66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z35" sqref="Z35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>